<commit_message>
Include sanity check for full load hours
</commit_message>
<xml_diff>
--- a/inputs/tariff_configuration_ALL.xlsx
+++ b/inputs/tariff_configuration_ALL.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\koch_j0\AMIRIS\demand_response_analyses_workflow\inputs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DBC07B2B-A550-45BC-811C-6C04F4B7AD69}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{39DFB570-3EA2-4DC6-83AF-0E2F18AA7678}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="38400" windowHeight="17625" activeTab="1" xr2:uid="{3118DBBB-A8B8-40F0-B654-F617A01C8433}"/>
   </bookViews>
@@ -1164,7 +1164,7 @@
   <dimension ref="A1:F18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A9" sqref="A9"/>
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Add minor changes in tariffs configuration Excel workbook
</commit_message>
<xml_diff>
--- a/inputs/tariff_configuration_ALL.xlsx
+++ b/inputs/tariff_configuration_ALL.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\koch_j0\AMIRIS\demand_response_analyses_workflow\inputs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BE2F3C5A-6F24-41EF-AC99-13699DAEB753}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8BBAAD7C-0798-49CE-A0CC-DC12085B7240}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="38400" windowHeight="17625" xr2:uid="{3118DBBB-A8B8-40F0-B654-F617A01C8433}"/>
   </bookViews>
@@ -433,8 +433,9 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="1">
+  <numFmts count="2">
     <numFmt numFmtId="164" formatCode="0.0"/>
+    <numFmt numFmtId="165" formatCode="0.000"/>
   </numFmts>
   <fonts count="13" x14ac:knownFonts="1">
     <font>
@@ -584,7 +585,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="30">
+  <cellXfs count="31">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -631,6 +632,7 @@
     </xf>
     <xf numFmtId="0" fontId="12" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="7" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Link" xfId="1" builtinId="8"/>
@@ -683,9 +685,9 @@
       <sheetName val="Multiplier_100_dyn_80_LP"/>
     </sheetNames>
     <sheetDataSet>
-      <sheetData sheetId="0"/>
-      <sheetData sheetId="1"/>
-      <sheetData sheetId="2"/>
+      <sheetData sheetId="0" refreshError="1"/>
+      <sheetData sheetId="1" refreshError="1"/>
+      <sheetData sheetId="2" refreshError="1"/>
       <sheetData sheetId="3">
         <row r="13">
           <cell r="I13">
@@ -693,30 +695,30 @@
           </cell>
         </row>
       </sheetData>
-      <sheetData sheetId="4"/>
-      <sheetData sheetId="5"/>
-      <sheetData sheetId="6"/>
-      <sheetData sheetId="7"/>
-      <sheetData sheetId="8"/>
-      <sheetData sheetId="9"/>
-      <sheetData sheetId="10"/>
-      <sheetData sheetId="11"/>
-      <sheetData sheetId="12"/>
-      <sheetData sheetId="13"/>
-      <sheetData sheetId="14"/>
-      <sheetData sheetId="15"/>
-      <sheetData sheetId="16"/>
-      <sheetData sheetId="17"/>
-      <sheetData sheetId="18"/>
-      <sheetData sheetId="19"/>
-      <sheetData sheetId="20"/>
-      <sheetData sheetId="21"/>
-      <sheetData sheetId="22"/>
-      <sheetData sheetId="23"/>
-      <sheetData sheetId="24"/>
-      <sheetData sheetId="25"/>
-      <sheetData sheetId="26"/>
-      <sheetData sheetId="27"/>
+      <sheetData sheetId="4" refreshError="1"/>
+      <sheetData sheetId="5" refreshError="1"/>
+      <sheetData sheetId="6" refreshError="1"/>
+      <sheetData sheetId="7" refreshError="1"/>
+      <sheetData sheetId="8" refreshError="1"/>
+      <sheetData sheetId="9" refreshError="1"/>
+      <sheetData sheetId="10" refreshError="1"/>
+      <sheetData sheetId="11" refreshError="1"/>
+      <sheetData sheetId="12" refreshError="1"/>
+      <sheetData sheetId="13" refreshError="1"/>
+      <sheetData sheetId="14" refreshError="1"/>
+      <sheetData sheetId="15" refreshError="1"/>
+      <sheetData sheetId="16" refreshError="1"/>
+      <sheetData sheetId="17" refreshError="1"/>
+      <sheetData sheetId="18" refreshError="1"/>
+      <sheetData sheetId="19" refreshError="1"/>
+      <sheetData sheetId="20" refreshError="1"/>
+      <sheetData sheetId="21" refreshError="1"/>
+      <sheetData sheetId="22" refreshError="1"/>
+      <sheetData sheetId="23" refreshError="1"/>
+      <sheetData sheetId="24" refreshError="1"/>
+      <sheetData sheetId="25" refreshError="1"/>
+      <sheetData sheetId="26" refreshError="1"/>
+      <sheetData sheetId="27" refreshError="1"/>
     </sheetDataSet>
   </externalBook>
 </externalLink>
@@ -1207,7 +1209,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D3B6F998-9ABC-4707-A766-B287B89607D5}">
   <dimension ref="A1:G18"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B1" sqref="B1"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -1970,9 +1974,11 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{78948DBB-3091-409B-A186-B130C0B79515}">
-  <dimension ref="A1:G18"/>
+  <dimension ref="A1:G19"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C19" sqref="C19"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -2341,8 +2347,11 @@
         <v>46</v>
       </c>
     </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" s="14"/>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C19" s="30"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>

</xml_diff>